<commit_message>
add reporte de matriz de confucion y normalizada a demas de curvas de aprendizaje, roc, etc
</commit_message>
<xml_diff>
--- a/reports/reportes_modelos.xlsx
+++ b/reports/reportes_modelos.xlsx
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8216560509554141</v>
+        <v>0.8152866242038217</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7704918032786885</v>
+        <v>0.768</v>
       </c>
       <c r="D2" t="n">
-        <v>0.734375</v>
+        <v>0.75</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8103448275862069</v>
+        <v>0.7868852459016393</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7707006369426752</v>
+        <v>0.8089171974522293</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7230769230769231</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="D3" t="n">
-        <v>0.734375</v>
+        <v>0.65625</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7121212121212122</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +506,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.802547770700637</v>
+        <v>0.8089171974522293</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7304347826086957</v>
+        <v>0.7413793103448276</v>
       </c>
       <c r="D4" t="n">
-        <v>0.65625</v>
+        <v>0.671875</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.8269230769230769</v>
       </c>
     </row>
     <row r="5">
@@ -619,13 +619,13 @@
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7961696306429549</v>
+        <v>0.7906976744186046</v>
       </c>
       <c r="G2" t="n">
+        <v>0.8343949044585988</v>
+      </c>
+      <c r="H2" t="n">
         <v>0.8152866242038217</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.8216560509554141</v>
       </c>
     </row>
     <row r="3">
@@ -649,13 +649,13 @@
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8426812585499316</v>
+        <v>0.8344733242134063</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8407643312101911</v>
+        <v>0.8152866242038217</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7707006369426752</v>
+        <v>0.8089171974522293</v>
       </c>
     </row>
     <row r="4">
@@ -679,13 +679,13 @@
         <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8358413132694938</v>
+        <v>0.8331053351573188</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8280254777070064</v>
+        <v>0.8343949044585988</v>
       </c>
       <c r="H4" t="n">
-        <v>0.802547770700637</v>
+        <v>0.8089171974522293</v>
       </c>
     </row>
     <row r="5">

</xml_diff>